<commit_message>
Ajuste en la descarga de excel en pantalla de inicio de reglas, visualizacion de claves de parametros.
Se agrega filtrado de entrega y años en pantalla de Reglas a validar
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/ResumenResultadosaValidarMonitoreo.xlsx
+++ b/WebAPI/wwwroot/Plantillas/ResumenResultadosaValidarMonitoreo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nrojast\Documents\Plantillas_cu6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6DB7B-C0F9-4672-BDBB-52EF9D4C7B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4296"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen a validar" sheetId="1" r:id="rId1"/>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,10 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,22 +419,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="P2" sqref="P2:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="15" max="15" width="14.44140625" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" customWidth="1"/>
-    <col min="20" max="20" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="99.140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Se hace ajsute en la descarga de informacion en la pantalla de inicio de reglas, se agregaron columnas al formato excel. Se crea vista para la obtener los resultados que no cumplieron con la fecha de entrega Se crean repositorios para consultar vista de vwResultadosNoCumplenFechaEntrega Se crea funcion en java script para regresar respuesta de dicha vista Ajuste en el fron en la columna de Observaciones se muestra la clave del parametro y no el numero de regla Se crea funcion para la descarga de excel con los parametros qu eno cumplieron con la fecha de entrega
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/ResumenResultadosaValidarMonitoreo.xlsx
+++ b/WebAPI/wwwroot/Plantillas/ResumenResultadosaValidarMonitoreo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nayeli Rojas\Documents\SICA_INFOTEC\WebAPI\wwwroot\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6DB7B-C0F9-4672-BDBB-52EF9D4C7B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen a validar" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Clave Sitio</t>
   </si>
@@ -78,19 +77,22 @@
     <t>Se corre reglas de validación</t>
   </si>
   <si>
-    <t>Autorización de reglas cuando esté incompleto. (SI)</t>
-  </si>
-  <si>
-    <t>Cumple con todos los criterios para aplicar reglas? (SI/NO)</t>
-  </si>
-  <si>
     <t>Diferencia en días</t>
+  </si>
+  <si>
+    <t>Cumple con todos los criterios para aplicar reglas?  (SI/NO)</t>
+  </si>
+  <si>
+    <t>Autorización de reglas cuando esté incompleto (SI/NO)</t>
+  </si>
+  <si>
+    <t>Autorización de reglas cuando no cumple fecha de entrega (SI/NO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,6 +102,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -132,13 +135,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,84 +425,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="99.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" customWidth="1"/>
+    <col min="1" max="14" width="11.44140625" style="1"/>
+    <col min="15" max="15" width="14.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="96" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="23.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="21.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="27.109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>